<commit_message>
Port connected, ready to send flits into router
</commit_message>
<xml_diff>
--- a/HW3/hw3/EXAMPLE1.xlsx
+++ b/HW3/hw3/EXAMPLE1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacky\Desktop\NoC\HW3\hw3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5201612-43C8-4C20-ADB3-A4D0F461415C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACD89D8-F89C-4E99-BABB-F2626F59D58C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-13068" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{62D3B6F3-6DD7-4864-92F9-5938D6DC688C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{62D3B6F3-6DD7-4864-92F9-5938D6DC688C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="91">
-  <si>
-    <t>Source routing for core0</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="103">
   <si>
     <t>Destination</t>
   </si>
@@ -180,9 +177,6 @@
     <t>Send 73 values to core 10</t>
   </si>
   <si>
-    <t>Source routing for core11</t>
-  </si>
-  <si>
     <t>Core_11.txt</t>
   </si>
   <si>
@@ -310,6 +304,48 @@
   </si>
   <si>
     <t>Create the router with buffer size of 5 for each N,S,E,W,X ports, no virtual channel</t>
+  </si>
+  <si>
+    <t>Uses algorithmic routing</t>
+  </si>
+  <si>
+    <t>Source routing for core0-&gt;10</t>
+  </si>
+  <si>
+    <t>Source routing for core11-&gt;0</t>
+  </si>
+  <si>
+    <t>sx</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>sy</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>sx = 0 means positive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sy = 1 means negative </t>
+  </si>
+  <si>
+    <t>First move x,then move y</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>14%4=2</t>
+  </si>
+  <si>
+    <t>14/4=3</t>
+  </si>
+  <si>
+    <t>Note axes, if x positive go south, if y positive go east</t>
   </si>
 </sst>
 </file>
@@ -400,20 +436,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,7 +479,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>593053</xdr:colOff>
+      <xdr:colOff>591783</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>151910</xdr:rowOff>
     </xdr:to>
@@ -488,7 +525,7 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>2323430</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>176089</xdr:rowOff>
+      <xdr:rowOff>174819</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -530,9 +567,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>2284957</xdr:colOff>
+      <xdr:colOff>2284958</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>139590</xdr:rowOff>
+      <xdr:rowOff>138320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -934,17 +971,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C68AC21-3F7C-4DBE-9401-9EFC66F411A3}">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView zoomScale="101" zoomScaleNormal="101" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.26953125" customWidth="1"/>
-    <col min="3" max="3" width="22.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.36328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="1.90625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="35.54296875" bestFit="1" customWidth="1"/>
@@ -955,73 +992,76 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="N1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>102</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>51</v>
+        <v>17</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="K3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4">
@@ -1038,10 +1078,10 @@
       </c>
       <c r="J4" s="4"/>
       <c r="K4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="O4">
         <v>1</v>
@@ -1049,22 +1089,22 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="5">
+        <v>51</v>
+      </c>
+      <c r="E5" s="10">
         <v>0</v>
       </c>
       <c r="N5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O5">
         <v>5</v>
@@ -1072,132 +1112,132 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="5"/>
+        <v>52</v>
+      </c>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E9" s="4">
         <v>1</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>26</v>
+      <c r="A10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E10" s="4"/>
       <c r="K10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E11" s="4"/>
       <c r="K11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>11</v>
       </c>
-      <c r="D12" t="s">
-        <v>60</v>
-      </c>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A13" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" t="s">
-        <v>12</v>
-      </c>
       <c r="D13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E13" s="4">
         <v>2</v>
@@ -1205,46 +1245,46 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E16" s="4">
         <v>3</v>
@@ -1252,138 +1292,197 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="G19" t="s">
+        <v>93</v>
+      </c>
+      <c r="H19" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
+        <v>76</v>
+      </c>
+      <c r="F20" t="s">
+        <v>99</v>
+      </c>
+      <c r="G20" t="s">
+        <v>100</v>
+      </c>
+      <c r="H20" t="s">
+        <v>101</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="L20" s="6"/>
+      <c r="N20" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="K20" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="L20" s="7"/>
-      <c r="N20" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="O20" s="7"/>
+      <c r="O20" s="6"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="K21" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="L21" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="N21" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="O21" s="6" t="s">
-        <v>51</v>
+        <v>41</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N21" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="O21" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="K22" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="L22" s="6">
+        <v>42</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="L22" s="5">
         <v>0.18648600000000001</v>
       </c>
-      <c r="N22" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="O22" s="6">
+      <c r="N22" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="O22" s="5">
         <v>0.87162600000000001</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K23" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="L23" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="N23" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="O23" s="6" t="s">
-        <v>73</v>
+        <v>17</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="N23" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="O23" s="5" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="K24" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="L24" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="N24" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="O24" s="6" t="s">
-        <v>77</v>
+      <c r="A24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="N24" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O24" s="5" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="K25" s="8" t="s">
-        <v>81</v>
+      <c r="A25" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" t="s">
+        <v>95</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1419,7 +1518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6882F1ED-52BE-4DA4-AE35-87BBDD9E32C7}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1430,7 +1529,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -1438,15 +1537,15 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>90</v>
+      <c r="B3" s="9" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -1454,7 +1553,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -1462,7 +1561,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -1470,7 +1569,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -1478,7 +1577,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Core to router fifo done, start simulating buffer stuck condition
</commit_message>
<xml_diff>
--- a/HW3/hw3/EXAMPLE1.xlsx
+++ b/HW3/hw3/EXAMPLE1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacky\Desktop\NoC\HW3\hw3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACD89D8-F89C-4E99-BABB-F2626F59D58C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6458F404-E4F2-413C-9293-47EF84EB5A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{62D3B6F3-6DD7-4864-92F9-5938D6DC688C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="103">
   <si>
     <t>Destination</t>
   </si>
@@ -447,10 +447,10 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -974,7 +974,7 @@
   <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1014,7 +1014,7 @@
       <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>102</v>
       </c>
       <c r="K2" s="1" t="s">
@@ -1076,7 +1076,9 @@
       <c r="I4" s="4">
         <v>3</v>
       </c>
-      <c r="J4" s="4"/>
+      <c r="J4" s="4" t="s">
+        <v>93</v>
+      </c>
       <c r="K4" t="s">
         <v>45</v>
       </c>
@@ -1100,7 +1102,7 @@
       <c r="D5" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="11">
         <v>0</v>
       </c>
       <c r="N5" t="s">
@@ -1123,7 +1125,7 @@
       <c r="D6" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="10"/>
+      <c r="E6" s="11"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -1318,7 +1320,9 @@
       <c r="D18" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="4"/>
+      <c r="E18" s="4" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">

</xml_diff>